<commit_message>
Building EI XML insert scripts
</commit_message>
<xml_diff>
--- a/Spreadsheet/Current Mapping/20190304 LDB to LEMIR E_I_Mapping Sharon 3rd update.xlsx
+++ b/Spreadsheet/Current Mapping/20190304 LDB to LEMIR E_I_Mapping Sharon 3rd update.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\FromLB\Sharon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\source\repos\solid-waste-migration\Spreadsheet\Current Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70EA3BD-F5BB-4170-957B-B371E8334E30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2E8838-48EA-434E-AC57-A70FFC703921}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1150,7 +1150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1201,9 +1201,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1221,6 +1218,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1321,6 +1325,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:F51" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A2:F51" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:F51">
+    <sortCondition ref="A2:A51"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="LEMIR Type from righthand table" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="LDB_FacilityType"/>
@@ -1634,7 +1641,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,20 +1659,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="5"/>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1701,19 +1708,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H3" s="2">
         <v>10041</v>
@@ -1730,19 +1737,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H4" s="2">
         <v>10042</v>
@@ -1759,19 +1766,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H5" s="2">
         <v>10043</v>
@@ -1788,19 +1795,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H6" s="2">
         <v>10044</v>
@@ -1817,19 +1824,19 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H7" s="2">
         <v>10045</v>
@@ -1846,19 +1853,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H8" s="2">
         <v>10046</v>
@@ -1873,21 +1880,24 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="H9" s="2">
         <v>10047</v>
@@ -1902,24 +1912,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>117</v>
+        <v>295</v>
       </c>
       <c r="H10" s="2">
         <v>10048</v>
@@ -1936,19 +1946,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
+        <v>97</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="H11" s="2">
         <v>10049</v>
@@ -1965,19 +1969,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>4</v>
+        <v>94</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="H12" s="2">
         <v>10050</v>
@@ -1994,13 +1992,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>114</v>
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
       </c>
       <c r="H13" s="2">
         <v>10051</v>
@@ -2017,13 +2021,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>115</v>
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
       </c>
       <c r="H14" s="2">
         <v>10052</v>
@@ -2040,19 +2050,19 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="H15" s="2">
         <v>10053</v>
@@ -2069,19 +2079,19 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H16" s="2">
         <v>10054</v>
@@ -2098,13 +2108,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>41</v>
+        <v>296</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -2127,13 +2137,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>88</v>
+        <v>297</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -2156,13 +2166,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>72</v>
+        <v>297</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -2185,13 +2195,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>72</v>
+        <v>297</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -2200,15 +2210,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>40</v>
+        <v>297</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>
@@ -2216,36 +2226,36 @@
       <c r="E21" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>88</v>
+        <v>297</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>14</v>
+        <v>297</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -2256,13 +2266,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>14</v>
+        <v>297</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
         <v>4</v>
@@ -2271,44 +2281,38 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D25" t="s">
         <v>4</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2316,27 +2320,30 @@
         <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
         <v>4</v>
@@ -2345,72 +2352,69 @@
         <v>4</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
         <v>4</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="E31" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D32" t="s">
         <v>4</v>
@@ -2421,64 +2425,67 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
       </c>
       <c r="E34" t="s">
         <v>4</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D36" t="s">
         <v>4</v>
@@ -2489,13 +2496,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>297</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
@@ -2506,13 +2513,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>297</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -2521,15 +2528,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>297</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
@@ -2537,16 +2544,19 @@
       <c r="E39" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="F39" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>297</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
@@ -2555,18 +2565,18 @@
         <v>4</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>299</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
@@ -2577,65 +2587,64 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>297</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B43" t="s">
         <v>59</v>
       </c>
-      <c r="C42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" t="s">
-        <v>4</v>
-      </c>
-      <c r="E42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>303</v>
+      <c r="C43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>297</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>3</v>
       </c>
       <c r="D45" t="s">
         <v>4</v>
@@ -2644,35 +2653,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
         <v>4</v>
       </c>
       <c r="E46" t="s">
         <v>4</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="D47" t="s">
         <v>4</v>
@@ -2683,13 +2689,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D48" t="s">
         <v>4</v>
@@ -2698,15 +2704,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="B49" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D49" t="s">
         <v>4</v>
@@ -2715,38 +2721,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D50" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B51" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" t="s">
         <v>73</v>
       </c>
-      <c r="D51" t="s">
-        <v>72</v>
-      </c>
-      <c r="E51" t="s">
-        <v>73</v>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
+      <c r="B51" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -2771,7 +2778,7 @@
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="A10" sqref="A10:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2831,19 +2838,19 @@
       <c r="M1" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="N1" s="24" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>135</v>
@@ -2861,39 +2868,39 @@
         <v>141</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="M2" s="12">
-        <v>38412</v>
+        <v>41176</v>
       </c>
       <c r="N2" s="22" t="s">
-        <v>172</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>179</v>
+        <v>252</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>180</v>
+        <v>253</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>13</v>
@@ -2902,39 +2909,39 @@
         <v>1</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>182</v>
+        <v>254</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="M3" s="12">
-        <v>35317</v>
-      </c>
-      <c r="N3" s="22" t="s">
-        <v>172</v>
+        <v>28317</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>184</v>
+        <v>255</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>185</v>
+        <v>256</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>59</v>
@@ -2946,42 +2953,42 @@
         <v>1</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>186</v>
+        <v>257</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>187</v>
+        <v>258</v>
       </c>
       <c r="M4" s="12">
-        <v>38888</v>
-      </c>
-      <c r="N4" s="22" t="s">
-        <v>172</v>
+        <v>30949</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>188</v>
+        <v>264</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>189</v>
+        <v>265</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>13</v>
@@ -2993,36 +3000,34 @@
         <v>141</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>190</v>
+        <v>266</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>191</v>
+        <v>267</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="M5" s="12">
-        <v>33190</v>
-      </c>
+        <v>268</v>
+      </c>
+      <c r="M5" s="26"/>
       <c r="N5" s="23" t="s">
-        <v>83</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>193</v>
+        <v>269</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>194</v>
+        <v>270</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>145</v>
+        <v>271</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>59</v>
@@ -3034,23 +3039,23 @@
         <v>1</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>195</v>
+        <v>272</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>196</v>
+        <v>273</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>197</v>
+        <v>274</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="23" t="s">
-        <v>41</v>
+        <v>298</v>
       </c>
       <c r="O6" s="15" t="s">
         <v>198</v>
@@ -3058,16 +3063,16 @@
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>199</v>
+        <v>275</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>200</v>
+        <v>276</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>59</v>
@@ -3082,39 +3087,37 @@
         <v>141</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>201</v>
+        <v>277</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="M7" s="12">
-        <v>41176</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="M7" s="26"/>
       <c r="N7" s="23" t="s">
-        <v>9</v>
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>205</v>
+        <v>280</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>137</v>
+        <v>239</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>13</v>
@@ -3126,22 +3129,20 @@
         <v>141</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>207</v>
+        <v>281</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>208</v>
+        <v>241</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="M8" s="12">
-        <v>36378</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="M8" s="26"/>
       <c r="N8" s="23" t="s">
-        <v>172</v>
+        <v>298</v>
       </c>
       <c r="O8" s="14" t="s">
         <v>210</v>
@@ -3149,63 +3150,61 @@
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>211</v>
+        <v>283</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>212</v>
+        <v>284</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>137</v>
+        <v>285</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>213</v>
+        <v>286</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>164</v>
+        <v>287</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="M9" s="12">
-        <v>36672</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="M9" s="26"/>
       <c r="N9" s="23" t="s">
-        <v>172</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>215</v>
+        <v>174</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>13</v>
@@ -3214,39 +3213,39 @@
         <v>1</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="M10" s="12">
-        <v>34297</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>83</v>
+        <v>38412</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>220</v>
+        <v>166</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>181</v>
@@ -3261,22 +3260,22 @@
         <v>141</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>222</v>
+        <v>167</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="M11" s="12">
-        <v>38699</v>
-      </c>
-      <c r="N11" s="23" t="s">
-        <v>83</v>
+        <v>35317</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>172</v>
       </c>
       <c r="O11" s="14" t="s">
         <v>290</v>
@@ -3284,13 +3283,13 @@
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>225</v>
+        <v>185</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>135</v>
@@ -3308,39 +3307,39 @@
         <v>141</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>226</v>
+        <v>186</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>227</v>
+        <v>187</v>
       </c>
       <c r="M12" s="12">
-        <v>40158</v>
-      </c>
-      <c r="N12" s="23" t="s">
+        <v>38888</v>
+      </c>
+      <c r="N12" s="21" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>135</v>
+        <v>206</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>13</v>
@@ -3352,69 +3351,83 @@
         <v>141</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="M13" s="12">
-        <v>40630</v>
-      </c>
-      <c r="N13" s="23" t="s">
+        <v>36378</v>
+      </c>
+      <c r="N13" s="22" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="18" t="s">
+      <c r="A14" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="23" t="s">
-        <v>83</v>
+      <c r="G14" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="M14" s="12">
+        <v>36672</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>135</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>13</v>
@@ -3426,33 +3439,33 @@
         <v>141</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>235</v>
+        <v>146</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="M15" s="12">
-        <v>37169</v>
-      </c>
-      <c r="N15" s="23" t="s">
+        <v>40158</v>
+      </c>
+      <c r="N15" s="22" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>239</v>
+        <v>149</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>135</v>
@@ -3470,39 +3483,39 @@
         <v>141</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>241</v>
+        <v>150</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="M16" s="12">
-        <v>38793</v>
-      </c>
-      <c r="N16" s="23" t="s">
+        <v>40630</v>
+      </c>
+      <c r="N16" s="22" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>135</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>13</v>
@@ -3514,39 +3527,39 @@
         <v>141</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>155</v>
+        <v>235</v>
       </c>
       <c r="K17" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>154</v>
+        <v>236</v>
       </c>
       <c r="M17" s="12">
-        <v>38198</v>
-      </c>
-      <c r="N17" s="23" t="s">
+        <v>37169</v>
+      </c>
+      <c r="N17" s="22" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>135</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>13</v>
@@ -3558,36 +3571,36 @@
         <v>141</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="M18" s="12">
-        <v>35683</v>
-      </c>
-      <c r="N18" s="23" t="s">
+        <v>38793</v>
+      </c>
+      <c r="N18" s="22" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>59</v>
@@ -3599,25 +3612,25 @@
         <v>1</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K19" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M19" s="12">
-        <v>28317</v>
-      </c>
-      <c r="N19" s="24" t="s">
-        <v>298</v>
+        <v>38198</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="O19" s="14" t="s">
         <v>291</v>
@@ -3625,19 +3638,19 @@
     </row>
     <row r="20" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>156</v>
+        <v>248</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>13</v>
@@ -3646,25 +3659,25 @@
         <v>1</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>157</v>
+        <v>250</v>
       </c>
       <c r="K20" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="M20" s="12">
-        <v>30949</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>298</v>
+        <v>35683</v>
+      </c>
+      <c r="N20" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="O20" s="14" t="s">
         <v>291</v>
@@ -3708,25 +3721,25 @@
         <v>263</v>
       </c>
       <c r="M21" s="13"/>
-      <c r="N21" s="23" t="s">
+      <c r="N21" s="22" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>264</v>
+        <v>193</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>265</v>
+        <v>194</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>13</v>
@@ -3738,34 +3751,34 @@
         <v>141</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>266</v>
+        <v>195</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>267</v>
+        <v>196</v>
       </c>
       <c r="K22" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>268</v>
+        <v>197</v>
       </c>
       <c r="M22" s="13"/>
-      <c r="N22" s="24" t="s">
-        <v>298</v>
+      <c r="N22" s="22" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>269</v>
+        <v>188</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>270</v>
+        <v>189</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>271</v>
+        <v>144</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>59</v>
@@ -3777,23 +3790,25 @@
         <v>1</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="K23" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>274</v>
-      </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="24" t="s">
-        <v>298</v>
+        <v>192</v>
+      </c>
+      <c r="M23" s="27">
+        <v>33190</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="O23" s="15" t="s">
         <v>292</v>
@@ -3801,19 +3816,19 @@
     </row>
     <row r="24" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>275</v>
+        <v>214</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>276</v>
+        <v>215</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="F24" s="10" t="s">
         <v>13</v>
@@ -3822,23 +3837,25 @@
         <v>1</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>277</v>
+        <v>216</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="K24" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="M24" s="13"/>
-      <c r="N24" s="24" t="s">
-        <v>298</v>
+        <v>217</v>
+      </c>
+      <c r="M24" s="27">
+        <v>34297</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="O24" s="15" t="s">
         <v>293</v>
@@ -3846,19 +3863,19 @@
     </row>
     <row r="25" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>279</v>
+        <v>218</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>280</v>
+        <v>219</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>59</v>
+        <v>181</v>
       </c>
       <c r="F25" s="10" t="s">
         <v>13</v>
@@ -3870,72 +3887,66 @@
         <v>141</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>281</v>
+        <v>221</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>241</v>
+        <v>222</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>134</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="M25" s="13"/>
-      <c r="N25" s="24" t="s">
-        <v>298</v>
+        <v>223</v>
+      </c>
+      <c r="M25" s="27">
+        <v>38699</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="O25" s="15" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="E26" s="10" t="s">
+      <c r="A26" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="E26" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>168</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="J26" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="L26" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="M26" s="13"/>
-      <c r="N26" s="24" t="s">
-        <v>298</v>
+      <c r="G26" s="19"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="O26" s="15" t="s">
         <v>294</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N26" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:N26" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N26">
+      <sortCondition ref="N1:N26"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>